<commit_message>
comenzando pruebas con lexer/parser dinamico que permita anidamientos condicionales
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas - copia.xlsx
+++ b/Final/dominio/formulas - copia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>tag</t>
   </si>
@@ -53,8 +53,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,6 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -443,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>7.15</v>
+        <v>2.1</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
@@ -464,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>7.15</v>
+        <v>2.1</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
@@ -485,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>7.15</v>
+        <v>2.1</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>
@@ -521,6 +530,51 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(AND(B6&gt;3,B6&lt;7),"presion no estable","presion estable")</f>
+        <v>presion no estable</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(OR(B7&lt;3,B7&gt;7),"presion no estable","presion estable")</f>
+        <v>presion estable</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
agregando visualizador al nodo para ver los datos cargados desde planilla, se hizo el marco, todavia no muestra datos
</commit_message>
<xml_diff>
--- a/Final/dominio/formulas - copia.xlsx
+++ b/Final/dominio/formulas - copia.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Hoja1" state="show" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -52,22 +52,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +90,9 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -413,11 +415,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="1" customWidth="1"/>
@@ -452,14 +454,14 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>2.1</v>
+        <v>7.45</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2&gt;C2,"green","blue")</f>
-        <v>blue</v>
+        <v>green</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -473,14 +475,14 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>2.1</v>
+        <v>7.45</v>
       </c>
       <c r="C3" s="1">
         <v>3.5</v>
       </c>
       <c r="D3" t="str">
         <f>IF(B3&gt;=C3,"red","yellow")</f>
-        <v>yellow</v>
+        <v>red</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -494,14 +496,14 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>2.1</v>
+        <v>7.45</v>
       </c>
       <c r="C4" s="1">
         <v>6.8</v>
       </c>
       <c r="D4" t="str">
         <f>IF(B4&gt;C4,"presion alta","presion normal")</f>
-        <v>presion normal</v>
+        <v>presion alta</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -512,23 +514,23 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>7.45</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>6.8</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(B5=C5,"green","blue")</f>
-        <v>green</v>
+        <f>IF(AND(B5&gt;3,B5&lt;7),"presion alta","presion normal")</f>
+        <v>presion normal</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -542,8 +544,8 @@
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(AND(B6&gt;3,B6&lt;7),"presion no estable","presion estable")</f>
-        <v>presion no estable</v>
+        <f>IF(B6=C6,"green","blue")</f>
+        <v>blue</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -563,8 +565,8 @@
         <v>1</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(OR(B7&lt;3,B7&gt;7),"presion no estable","presion estable")</f>
-        <v>presion estable</v>
+        <f>IF(AND(B7&gt;3,B7&lt;7),"marcha combinada","marcha no combinada")</f>
+        <v>marcha no combinada</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
@@ -573,11 +575,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>